<commit_message>
update template soal excel
</commit_message>
<xml_diff>
--- a/public/template-soal.xlsx
+++ b/public/template-soal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\labko\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projek\tes_online_unsika\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{98107300-C815-4088-8694-2B8BA1B140EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F60A9CD-81E7-4F7C-A378-2E486D269A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0A9E7554-5B29-4F5A-A64A-34063A3B2A3D}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>jenis_soal</t>
   </si>
@@ -74,6 +74,27 @@
   </si>
   <si>
     <t>dsksjfiwhdiuweu</t>
+  </si>
+  <si>
+    <t>multi_choice</t>
+  </si>
+  <si>
+    <t>Lorem ipsum?</t>
+  </si>
+  <si>
+    <t>hsdbfu</t>
+  </si>
+  <si>
+    <t>yuegwruy</t>
+  </si>
+  <si>
+    <t>uyweg</t>
+  </si>
+  <si>
+    <t>weyrgwey</t>
+  </si>
+  <si>
+    <t>a,b,d</t>
   </si>
 </sst>
 </file>
@@ -581,7 +602,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -940,7 +961,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,14 +1047,30 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>

</xml_diff>